<commit_message>
add check is_deleted of user == false or not
</commit_message>
<xml_diff>
--- a/src/services/excel/templates/import-admin-template.xlsx
+++ b/src/services/excel/templates/import-admin-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\SchoolMedix_BE\src\services\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458A2712-CE24-45BA-848C-C1A8659D77F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD3BA77-B99A-48D8-B5F2-3412D643DA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3810" yWindow="2925" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Nguyễn Văn A</t>
   </si>
@@ -91,6 +91,33 @@
   </si>
   <si>
     <t>Số 4 Phố Cổ Huế</t>
+  </si>
+  <si>
+    <t>fdsa@gmail.com</t>
+  </si>
+  <si>
+    <t>Kim Jong Un</t>
+  </si>
+  <si>
+    <t>Kim Ji Jok</t>
+  </si>
+  <si>
+    <t>Lee Chong Whey</t>
+  </si>
+  <si>
+    <t>Số 5 Ngô Tất Tố</t>
+  </si>
+  <si>
+    <t>Địa bàn Phường Nam Nha Trang</t>
+  </si>
+  <si>
+    <t>Địa bàn Phường Bắc Từ Liêm</t>
+  </si>
+  <si>
+    <t>aS@gmail.com</t>
+  </si>
+  <si>
+    <t>hi@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -100,10 +127,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,10 +161,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -146,8 +182,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +575,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -544,9 +584,78 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="F9" s="5"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{E84CA798-DEA1-4479-AB2F-98C72A5B06E3}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{720F92DB-6631-4066-BCCE-95794E924C07}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{1442A799-C2F0-4BA9-81AE-2381306D45FC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <ignoredErrors>
     <ignoredError sqref="F2:F3" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
finalize the import export excel of user feature
</commit_message>
<xml_diff>
--- a/src/services/excel/templates/import-admin-template.xlsx
+++ b/src/services/excel/templates/import-admin-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\SchoolMedix_BE\src\services\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD3BA77-B99A-48D8-B5F2-3412D643DA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268334C3-2DD0-4AB8-9C71-179439F533C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="2925" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="3270" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADMIN" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Nguyễn Văn A</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Nguyễn Văn C</t>
   </si>
   <si>
-    <t>14/03/2000</t>
-  </si>
-  <si>
-    <t>20/11/1993</t>
-  </si>
-  <si>
     <t>0362718422</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
   </si>
   <si>
     <t>Trần Thị D</t>
-  </si>
-  <si>
-    <t>20/11/1990</t>
   </si>
   <si>
     <t>asdffd@gmail.com</t>
@@ -124,8 +115,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-1010000]yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -165,7 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -184,6 +176,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -466,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,22 +479,22 @@
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="J1"/>
       <c r="K1"/>
@@ -514,34 +509,34 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
+      <c r="C2" s="7">
+        <v>36598</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+      <c r="C3" s="7">
+        <v>34113</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -551,102 +546,370 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
-        <v>32479</v>
+      <c r="C4" s="7">
+        <v>36598</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="7">
+        <v>34113</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="7">
+        <v>36598</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="7">
+        <v>36598</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="7">
+        <v>34113</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="7"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="7"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="7"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="7"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="7"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="7"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="7"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="7"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="7"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="7"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="7"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="7"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>